<commit_message>
Merge in 5/31 changes from Elizabeth Mahon, primarily focusing on full implementation of FillRegression() statistics.  Because she modified some other commands, in particular related to handling precision for numeric comparisons, there are also a few changes outside of FillRegression().
git-svn-id: file:///cygdrive/C/owf-svnrepos/TSTool-test/java_142/trunk@906 fa08ced2-b08f-4ccc-859c-2e92e4a1381a
</commit_message>
<xml_diff>
--- a/test/regression/commands/general/FillRegression/ExpectedResults/Test_FillRegression_Streamflow_Month_MonthlyEquations_excel.xlsx
+++ b/test/regression/commands/general/FillRegression/ExpectedResults/Test_FillRegression_Streamflow_Month_MonthlyEquations_excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="553">
   <si>
     <t>1997-01</t>
   </si>
@@ -1660,22 +1660,22 @@
     <t>No</t>
   </si>
   <si>
+    <t>Still an incomplete test; many values are just filled in due to me not knowing how best to do them in Excel.</t>
+  </si>
+  <si>
+    <t>However, it tests all of the math.</t>
+  </si>
+  <si>
+    <t>It's probably not as efficient as it could be, either - the cells used in said calculations were picked by hand from the Data sheet.</t>
+  </si>
+  <si>
     <t>Calc sheet is all of the tests - the equations and such.</t>
   </si>
   <si>
+    <t>Final is where I've been doing copy -&gt; paste value to make sure that it can be read. I didn't actually see if it would work without that, since it's a simple step.</t>
+  </si>
+  <si>
     <t>Data sheet is the independent time series (B), copied from the CSV, the dependent time series (C ), copied from the CSV, and the estimated values for the dependent (D), calculated using B and values in "calc".</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Final is where to copy as value the results, since TSTool can have problems evaluating the formulas.</t>
-  </si>
-  <si>
-    <t>Settings specified in the command (e.g. transformation type) need to be entered by hand.</t>
-  </si>
-  <si>
-    <t>Some values were entered by hand due to the difficulty of having Excel check values only every 12 rows.</t>
   </si>
 </sst>
 </file>
@@ -2020,37 +2020,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>552</v>
+        <v>548</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -2063,7 +2068,7 @@
   <dimension ref="A1:D156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3977,8 +3982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:NI18"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5173,32 +5178,23 @@
       <c r="C2" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D2" s="1" t="str">
-        <f>Data!A1</f>
-        <v>1997-01</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f>Data!A156</f>
-        <v>2009-12</v>
-      </c>
-      <c r="F2" s="1" t="str">
-        <f>Data!A1</f>
-        <v>1997-01</v>
-      </c>
-      <c r="G2" s="1" t="str">
-        <f>Data!A156</f>
-        <v>2009-12</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <f>Data!A1</f>
-        <v>1997-01</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <f>Data!A156</f>
-        <v>2009-12</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>549</v>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="K2" s="1">
         <v>2</v>
@@ -5221,7 +5217,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="1">
-        <f>AVERAGE(Data!C13,Data!C25)</f>
+        <f>SUM(Data!C13,Data!C25)/2</f>
         <v>1386.4665</v>
       </c>
       <c r="U2" s="1">
@@ -5232,7 +5228,7 @@
         <v>5</v>
       </c>
       <c r="W2" s="1">
-        <f>AVERAGE(Data!C13,Data!C25,Data!C37,Data!C49,Data!C61)</f>
+        <f>SUM(Data!C13,Data!C25,Data!C37,Data!C49,Data!C61)/V2</f>
         <v>1582.8329799999999</v>
       </c>
       <c r="X2" s="1">
@@ -6961,7 +6957,7 @@
   <dimension ref="A1:NF1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7161,9 +7157,6 @@
       <c r="I1" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>549</v>
-      </c>
       <c r="K1" s="3">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Save Elizabeth Mahon's enhancements to FillRegression as of 2013-06-19.  These are in addition to changes submitted for 2013-05-31.
git-svn-id: file:///cygdrive/C/owf-svnrepos/TSTool-test/java_142/trunk@907 fa08ced2-b08f-4ccc-859c-2e92e4a1381a
</commit_message>
<xml_diff>
--- a/test/regression/commands/general/FillRegression/ExpectedResults/Test_FillRegression_Streamflow_Month_MonthlyEquations_excel.xlsx
+++ b/test/regression/commands/general/FillRegression/ExpectedResults/Test_FillRegression_Streamflow_Month_MonthlyEquations_excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="553">
   <si>
     <t>1997-01</t>
   </si>
@@ -1660,22 +1660,22 @@
     <t>No</t>
   </si>
   <si>
-    <t>Still an incomplete test; many values are just filled in due to me not knowing how best to do them in Excel.</t>
-  </si>
-  <si>
-    <t>However, it tests all of the math.</t>
-  </si>
-  <si>
-    <t>It's probably not as efficient as it could be, either - the cells used in said calculations were picked by hand from the Data sheet.</t>
-  </si>
-  <si>
     <t>Calc sheet is all of the tests - the equations and such.</t>
   </si>
   <si>
-    <t>Final is where I've been doing copy -&gt; paste value to make sure that it can be read. I didn't actually see if it would work without that, since it's a simple step.</t>
-  </si>
-  <si>
     <t>Data sheet is the independent time series (B), copied from the CSV, the dependent time series (C ), copied from the CSV, and the estimated values for the dependent (D), calculated using B and values in "calc".</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Final is where to copy as value the results, since TSTool can have problems evaluating the formulas.</t>
+  </si>
+  <si>
+    <t>Settings specified in the command (e.g. transformation type) need to be entered by hand.</t>
+  </si>
+  <si>
+    <t>Some values were entered by hand due to the difficulty of having Excel check values only every 12 rows.</t>
   </si>
 </sst>
 </file>
@@ -2020,42 +2020,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -2068,7 +2063,7 @@
   <dimension ref="A1:D156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D158" sqref="D158"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3982,8 +3977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:NI18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5178,23 +5173,32 @@
       <c r="C2" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>155</v>
+      <c r="D2" s="1" t="str">
+        <f>Data!A1</f>
+        <v>1997-01</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>Data!A156</f>
+        <v>2009-12</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>Data!A1</f>
+        <v>1997-01</v>
+      </c>
+      <c r="G2" s="1" t="str">
+        <f>Data!A156</f>
+        <v>2009-12</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>Data!A1</f>
+        <v>1997-01</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>Data!A156</f>
+        <v>2009-12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>549</v>
       </c>
       <c r="K2" s="1">
         <v>2</v>
@@ -5217,7 +5221,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="1">
-        <f>SUM(Data!C13,Data!C25)/2</f>
+        <f>AVERAGE(Data!C13,Data!C25)</f>
         <v>1386.4665</v>
       </c>
       <c r="U2" s="1">
@@ -5228,7 +5232,7 @@
         <v>5</v>
       </c>
       <c r="W2" s="1">
-        <f>SUM(Data!C13,Data!C25,Data!C37,Data!C49,Data!C61)/V2</f>
+        <f>AVERAGE(Data!C13,Data!C25,Data!C37,Data!C49,Data!C61)</f>
         <v>1582.8329799999999</v>
       </c>
       <c r="X2" s="1">
@@ -6957,7 +6961,7 @@
   <dimension ref="A1:NF1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7157,6 +7161,9 @@
       <c r="I1" s="2" t="s">
         <v>155</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>549</v>
+      </c>
       <c r="K1" s="3">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Commit FillRegression test cleanup from Elizabeth Mahon from 2013-08-02.  All of the FillRegression tests should now pass.  Those that do not may be old and need to be removed or disabled.
git-svn-id: file:///cygdrive/C/owf-svnrepos/TSTool-test/java_142/trunk@909 fa08ced2-b08f-4ccc-859c-2e92e4a1381a
</commit_message>
<xml_diff>
--- a/test/regression/commands/general/FillRegression/ExpectedResults/Test_FillRegression_Streamflow_Month_MonthlyEquations_excel.xlsx
+++ b/test/regression/commands/general/FillRegression/ExpectedResults/Test_FillRegression_Streamflow_Month_MonthlyEquations_excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="553">
   <si>
     <t>1997-01</t>
   </si>
@@ -1666,16 +1666,16 @@
     <t>Data sheet is the independent time series (B), copied from the CSV, the dependent time series (C ), copied from the CSV, and the estimated values for the dependent (D), calculated using B and values in "calc".</t>
   </si>
   <si>
+    <t>Final is where to copy as value the results, since TSTool can have problems evaluating the formulas.</t>
+  </si>
+  <si>
+    <t>Settings specified in the command (e.g. transformation type) need to be entered by hand.</t>
+  </si>
+  <si>
+    <t>Some values were entered by hand due to the difficulty of having Excel check values only every 12 rows.</t>
+  </si>
+  <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>Final is where to copy as value the results, since TSTool can have problems evaluating the formulas.</t>
-  </si>
-  <si>
-    <t>Settings specified in the command (e.g. transformation type) need to be entered by hand.</t>
-  </si>
-  <si>
-    <t>Some values were entered by hand due to the difficulty of having Excel check values only every 12 rows.</t>
   </si>
 </sst>
 </file>
@@ -2040,17 +2040,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -3977,8 +3977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:NI18"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5198,10 +5198,10 @@
         <v>2009-12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="K2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M2" s="1">
         <v>70</v>
@@ -5271,16 +5271,14 @@
         <f>SQRT(AF6/N2)</f>
         <v>4.5474735088646412E-13</v>
       </c>
-      <c r="AK2" s="1" t="str">
-        <f>IF(N2&gt;K2,"Yes","No")</f>
-        <v>No</v>
-      </c>
-      <c r="AL2" s="1" t="str">
-        <f>IF(N2&gt;=K2,"Yes","No")</f>
-        <v>Yes</v>
+      <c r="AK2" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>546</v>
       </c>
       <c r="AN2" s="1">
-        <f>IF(AK2="No",0,(V2-N2))</f>
+        <f>IF(OR(AK2="No",AL2 ="No"),0,(V2-N2))</f>
         <v>0</v>
       </c>
       <c r="AR2" s="1">
@@ -5348,13 +5346,11 @@
         <f>SQRT(SUMSQ(Data!C14-Data!D14,Data!C26-Data!D26)/AR2)</f>
         <v>1.5916157281026244E-12</v>
       </c>
-      <c r="BO2" s="1" t="str">
-        <f>IF(AR2&gt;K2,"Yes","No")</f>
-        <v>No</v>
-      </c>
-      <c r="BP2" s="1" t="str">
-        <f>IF(AR2&gt;=K2,"Yes","No")</f>
-        <v>Yes</v>
+      <c r="BO2" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="BP2" s="1" t="s">
+        <v>546</v>
       </c>
       <c r="BR2" s="1">
         <f>IF(BO2="No",0,(AR2-AU2))</f>
@@ -5446,8 +5442,8 @@
         <v>-0.55315042866539366</v>
       </c>
       <c r="CR2" s="1">
-        <f>_xlfn.T.INV(M2/100,BV2-2)</f>
-        <v>0.72654252800536079</v>
+        <f>ABS(_xlfn.T.INV((100 - M2)/200,BV2-2))</f>
+        <v>1.9626105055051506</v>
       </c>
       <c r="CS2" s="1" t="str">
         <f>IF(CQ2&gt;CR2,"Yes","No")</f>
@@ -5547,8 +5543,8 @@
         <v>0.56224372800727651</v>
       </c>
       <c r="DV2" s="1">
-        <f>_xlfn.T.INV(M2/100,CZ2-2)</f>
-        <v>0.58438972743981854</v>
+        <f>ABS(_xlfn.T.INV((100 - M2)/200,CZ2-2))</f>
+        <v>1.2497781050332251</v>
       </c>
       <c r="DW2" s="1" t="str">
         <f>IF(DU2&gt;DV2,"Yes","No")</f>
@@ -5648,8 +5644,8 @@
         <v>13.453122720745055</v>
       </c>
       <c r="EZ2" s="1">
-        <f>_xlfn.T.INV(M2/100,ED2-2)</f>
-        <v>0.61721339984836765</v>
+        <f>ABS(_xlfn.T.INV((100 - M2)/200,ED2-2))</f>
+        <v>1.3862065601673439</v>
       </c>
       <c r="FA2" s="1" t="str">
         <f>IF(EY2&gt;EZ2,"Yes","No")</f>
@@ -5761,8 +5757,8 @@
         <v>11.289602581333723</v>
       </c>
       <c r="GD2" s="1">
-        <f>_xlfn.T.INV(M2/100,FH2-2)</f>
-        <v>0.61721339984836765</v>
+        <f>ABS(_xlfn.T.INV((100 - M2)/200,FH2-2))</f>
+        <v>1.3862065601673439</v>
       </c>
       <c r="GE2" s="1" t="str">
         <f>IF(GC2&gt;GD2,"Yes","No")</f>
@@ -5874,8 +5870,8 @@
         <v>3.5540007993099589</v>
       </c>
       <c r="HH2" s="1">
-        <f>_xlfn.T.INV(M2/100,GL2-2)</f>
-        <v>0.58438972743981854</v>
+        <f>ABS(_xlfn.T.INV((100 - M2)/200,GL2-2))</f>
+        <v>1.2497781050332251</v>
       </c>
       <c r="HI2" s="1" t="str">
         <f>IF(HG2&gt;HH2,"Yes","No")</f>
@@ -5987,8 +5983,8 @@
         <v>23.581680920976332</v>
       </c>
       <c r="IL2" s="1">
-        <f>_xlfn.T.INV(M2/100,HP2-2)</f>
-        <v>0.58438972743981854</v>
+        <f>ABS(_xlfn.T.INV((100 - M2)/200,HP2-2))</f>
+        <v>1.2497781050332251</v>
       </c>
       <c r="IM2" s="1" t="str">
         <f>IF(IK2&gt;IL2,"Yes","No")</f>
@@ -6100,8 +6096,8 @@
         <v>5.3988200837587845</v>
       </c>
       <c r="JP2" s="1">
-        <f>_xlfn.T.INV(M2/100,IT2-2)</f>
-        <v>0.58438972743981854</v>
+        <f>ABS(_xlfn.T.INV((100 - M2)/200,IT2-2))</f>
+        <v>1.2497781050332251</v>
       </c>
       <c r="JQ2" s="1" t="str">
         <f>IF(JO2&gt;JP2,"Yes","No")</f>
@@ -6213,8 +6209,8 @@
         <v>2.4850540763851203</v>
       </c>
       <c r="KT2" s="1">
-        <f>_xlfn.T.INV(M2/100,JX2-2)</f>
-        <v>0.58438972743981854</v>
+        <f>ABS(_xlfn.T.INV((100 - M2)/200,JX2-2))</f>
+        <v>1.2497781050332251</v>
       </c>
       <c r="KU2" s="1" t="str">
         <f>IF(KS2&gt;KT2,"Yes","No")</f>
@@ -6326,8 +6322,8 @@
         <v>1.9107428825501551</v>
       </c>
       <c r="LX2" s="1">
-        <f>_xlfn.T.INV(M2/100,LB2-2)</f>
-        <v>0.61721339984836765</v>
+        <f>ABS(_xlfn.T.INV((100 - M2)/200,LB2-2))</f>
+        <v>1.3862065601673439</v>
       </c>
       <c r="LY2" s="1" t="str">
         <f>IF(LW2&gt;LX2,"Yes","No")</f>
@@ -6421,9 +6417,8 @@
       <c r="NC2" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="ND2" s="1" t="str">
-        <f>IF(MF2&gt;=K2,"Yes","No")</f>
-        <v>Yes</v>
+      <c r="ND2" s="1" t="s">
+        <v>546</v>
       </c>
       <c r="NF2" s="1">
         <f>IF(NC2="No",0,MI2)</f>
@@ -6961,7 +6956,7 @@
   <dimension ref="A1:NF1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7162,10 +7157,10 @@
         <v>155</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="K1" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M1" s="2">
         <v>70</v>
@@ -7228,7 +7223,7 @@
         <v>546</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>532</v>
+        <v>546</v>
       </c>
       <c r="AN1" s="2">
         <v>0</v>
@@ -7290,7 +7285,7 @@
         <v>546</v>
       </c>
       <c r="BP1" s="2" t="s">
-        <v>532</v>
+        <v>546</v>
       </c>
       <c r="BR1" s="2">
         <v>0</v>
@@ -7362,7 +7357,7 @@
         <v>-0.55315042866539366</v>
       </c>
       <c r="CR1" s="2">
-        <v>0.72654252800536079</v>
+        <v>1.9626105055051506</v>
       </c>
       <c r="CS1" s="2" t="s">
         <v>546</v>
@@ -7440,7 +7435,7 @@
         <v>0.56224372800727651</v>
       </c>
       <c r="DV1" s="2">
-        <v>0.58438972743981854</v>
+        <v>1.2497781050332251</v>
       </c>
       <c r="DW1" s="2" t="s">
         <v>546</v>
@@ -7518,7 +7513,7 @@
         <v>13.453122720745055</v>
       </c>
       <c r="EZ1" s="2">
-        <v>0.61721339984836765</v>
+        <v>1.3862065601673439</v>
       </c>
       <c r="FA1" s="2" t="s">
         <v>532</v>
@@ -7605,7 +7600,7 @@
         <v>11.289602581333723</v>
       </c>
       <c r="GD1" s="2">
-        <v>0.61721339984836765</v>
+        <v>1.3862065601673439</v>
       </c>
       <c r="GE1" s="2" t="s">
         <v>532</v>
@@ -7692,7 +7687,7 @@
         <v>3.5540007993099589</v>
       </c>
       <c r="HH1" s="2">
-        <v>0.58438972743981854</v>
+        <v>1.2497781050332251</v>
       </c>
       <c r="HI1" s="2" t="s">
         <v>532</v>
@@ -7779,7 +7774,7 @@
         <v>23.581680920976332</v>
       </c>
       <c r="IL1" s="2">
-        <v>0.58438972743981854</v>
+        <v>1.2497781050332251</v>
       </c>
       <c r="IM1" s="2" t="s">
         <v>532</v>
@@ -7866,7 +7861,7 @@
         <v>5.3988200837587845</v>
       </c>
       <c r="JP1" s="2">
-        <v>0.58438972743981854</v>
+        <v>1.2497781050332251</v>
       </c>
       <c r="JQ1" s="2" t="s">
         <v>532</v>
@@ -7953,7 +7948,7 @@
         <v>2.4850540763851203</v>
       </c>
       <c r="KT1" s="2">
-        <v>0.58438972743981854</v>
+        <v>1.2497781050332251</v>
       </c>
       <c r="KU1" s="2" t="s">
         <v>532</v>
@@ -8040,7 +8035,7 @@
         <v>1.9107428825501551</v>
       </c>
       <c r="LX1" s="2">
-        <v>0.61721339984836765</v>
+        <v>1.3862065601673439</v>
       </c>
       <c r="LY1" s="2" t="s">
         <v>532</v>
@@ -8115,7 +8110,7 @@
         <v>546</v>
       </c>
       <c r="ND1" s="2" t="s">
-        <v>532</v>
+        <v>546</v>
       </c>
       <c r="NF1" s="2">
         <v>0</v>

</xml_diff>